<commit_message>
AAdded more genres and mappings
</commit_message>
<xml_diff>
--- a/unique_genres.xlsx
+++ b/unique_genres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Documents\Uni\3. Sem\DS Projekt\Code_and_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32349677-1106-4792-B3C0-C185C87D435D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F6BFAC-0ECC-4776-9CD9-A3C594AA67B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="764">
   <si>
     <t>adult standards</t>
   </si>
@@ -1552,9 +1552,6 @@
     <t>https://en.wikipedia.org/wiki/Banjo_music</t>
   </si>
   <si>
-    <t xml:space="preserve">instrumental </t>
-  </si>
-  <si>
     <t>https://www.reddit.com/r/Music/comments/k6s0fs/whats_mellow_gold_as_a_music_genre/</t>
   </si>
   <si>
@@ -1649,6 +1646,675 @@
   </si>
   <si>
     <t>Quelle</t>
+  </si>
+  <si>
+    <t>cabaret</t>
+  </si>
+  <si>
+    <t>french indie pop</t>
+  </si>
+  <si>
+    <t>acoustic guitar cover</t>
+  </si>
+  <si>
+    <t>african-american classical</t>
+  </si>
+  <si>
+    <t>afroswing</t>
+  </si>
+  <si>
+    <t>alabama metal</t>
+  </si>
+  <si>
+    <t>alternative emo</t>
+  </si>
+  <si>
+    <t>alternative roots rock</t>
+  </si>
+  <si>
+    <t>american contemporary classical</t>
+  </si>
+  <si>
+    <t>ann arbor indie</t>
+  </si>
+  <si>
+    <t>asian american hip hop</t>
+  </si>
+  <si>
+    <t>avant-garde jazz</t>
+  </si>
+  <si>
+    <t>azonto</t>
+  </si>
+  <si>
+    <t>background jazz</t>
+  </si>
+  <si>
+    <t>balkan brass</t>
+  </si>
+  <si>
+    <t>bardcore</t>
+  </si>
+  <si>
+    <t>baroque</t>
+  </si>
+  <si>
+    <t>bass trap</t>
+  </si>
+  <si>
+    <t>bass trip</t>
+  </si>
+  <si>
+    <t>bay area hip hop</t>
+  </si>
+  <si>
+    <t>bedroom soul</t>
+  </si>
+  <si>
+    <t>belgian rock</t>
+  </si>
+  <si>
+    <t>bemani</t>
+  </si>
+  <si>
+    <t>bluegrass</t>
+  </si>
+  <si>
+    <t>bluegrass fiddle</t>
+  </si>
+  <si>
+    <t>bluegrass gospel</t>
+  </si>
+  <si>
+    <t>bmore</t>
+  </si>
+  <si>
+    <t>boogie-woogie</t>
+  </si>
+  <si>
+    <t>boston hardcore</t>
+  </si>
+  <si>
+    <t>boston hip hop</t>
+  </si>
+  <si>
+    <t>boston rock</t>
+  </si>
+  <si>
+    <t>bouncy house</t>
+  </si>
+  <si>
+    <t>brazilian reggae</t>
+  </si>
+  <si>
+    <t>british alternative rock</t>
+  </si>
+  <si>
+    <t>british modern classical</t>
+  </si>
+  <si>
+    <t>british orchestra</t>
+  </si>
+  <si>
+    <t>british singer-songwriter</t>
+  </si>
+  <si>
+    <t>brooklyn indie</t>
+  </si>
+  <si>
+    <t>canadian blues</t>
+  </si>
+  <si>
+    <t>canadian electronic</t>
+  </si>
+  <si>
+    <t>canadian psychedelic rock</t>
+  </si>
+  <si>
+    <t>cantautor</t>
+  </si>
+  <si>
+    <t>champeta</t>
+  </si>
+  <si>
+    <t>chicago house</t>
+  </si>
+  <si>
+    <t>christian hip hop</t>
+  </si>
+  <si>
+    <t>christmas instrumental</t>
+  </si>
+  <si>
+    <t>circuit</t>
+  </si>
+  <si>
+    <t>city pop</t>
+  </si>
+  <si>
+    <t>classic dubstep</t>
+  </si>
+  <si>
+    <t>classic j-rock</t>
+  </si>
+  <si>
+    <t>classic norwegian pop</t>
+  </si>
+  <si>
+    <t>classic persian pop</t>
+  </si>
+  <si>
+    <t>classic progressive house</t>
+  </si>
+  <si>
+    <t>classical cello</t>
+  </si>
+  <si>
+    <t>classify</t>
+  </si>
+  <si>
+    <t>comedy rap</t>
+  </si>
+  <si>
+    <t>comic metal</t>
+  </si>
+  <si>
+    <t>corrosion</t>
+  </si>
+  <si>
+    <t>cosmic american</t>
+  </si>
+  <si>
+    <t>coverchill</t>
+  </si>
+  <si>
+    <t>croatian pop</t>
+  </si>
+  <si>
+    <t>crust punk</t>
+  </si>
+  <si>
+    <t>cumbia</t>
+  </si>
+  <si>
+    <t>dalarna indie</t>
+  </si>
+  <si>
+    <t>dancefloor dnb</t>
+  </si>
+  <si>
+    <t>dansktop</t>
+  </si>
+  <si>
+    <t>dark clubbing</t>
+  </si>
+  <si>
+    <t>dark post-punk</t>
+  </si>
+  <si>
+    <t>dark rock</t>
+  </si>
+  <si>
+    <t>dark wave</t>
+  </si>
+  <si>
+    <t>deep eurodance</t>
+  </si>
+  <si>
+    <t>deep funk</t>
+  </si>
+  <si>
+    <t>deep house</t>
+  </si>
+  <si>
+    <t>deep new americana</t>
+  </si>
+  <si>
+    <t>deep progressive trance</t>
+  </si>
+  <si>
+    <t>deep tropical house</t>
+  </si>
+  <si>
+    <t>derby indie</t>
+  </si>
+  <si>
+    <t>detroit trap</t>
+  </si>
+  <si>
+    <t>didgeridoo</t>
+  </si>
+  <si>
+    <t>doom metal</t>
+  </si>
+  <si>
+    <t>dream trance</t>
+  </si>
+  <si>
+    <t>drum and bass</t>
+  </si>
+  <si>
+    <t>dusseldorf electronic</t>
+  </si>
+  <si>
+    <t>dutch trance</t>
+  </si>
+  <si>
+    <t>early reggae</t>
+  </si>
+  <si>
+    <t>early romantic era</t>
+  </si>
+  <si>
+    <t>early us punk</t>
+  </si>
+  <si>
+    <t>electric bass</t>
+  </si>
+  <si>
+    <t>electro house</t>
+  </si>
+  <si>
+    <t>elephant 6</t>
+  </si>
+  <si>
+    <t>enka</t>
+  </si>
+  <si>
+    <t>escape room</t>
+  </si>
+  <si>
+    <t>focus beats</t>
+  </si>
+  <si>
+    <t>french rock-and-roll</t>
+  </si>
+  <si>
+    <t>funk carioca</t>
+  </si>
+  <si>
+    <t>futurepop</t>
+  </si>
+  <si>
+    <t>futuristic swag</t>
+  </si>
+  <si>
+    <t>gabba</t>
+  </si>
+  <si>
+    <t>german melodeath</t>
+  </si>
+  <si>
+    <t>german metal</t>
+  </si>
+  <si>
+    <t>german rock</t>
+  </si>
+  <si>
+    <t>german soundtrack</t>
+  </si>
+  <si>
+    <t>ghanaian hip hop</t>
+  </si>
+  <si>
+    <t>gothic rock</t>
+  </si>
+  <si>
+    <t>grunge pop</t>
+  </si>
+  <si>
+    <t>harmonica jazz</t>
+  </si>
+  <si>
+    <t>hawaiian</t>
+  </si>
+  <si>
+    <t>hopebeat</t>
+  </si>
+  <si>
+    <t>house</t>
+  </si>
+  <si>
+    <t>hyphy</t>
+  </si>
+  <si>
+    <t>icelandic indie</t>
+  </si>
+  <si>
+    <t>indie pop rock</t>
+  </si>
+  <si>
+    <t>instrumental funk</t>
+  </si>
+  <si>
+    <t>j-pop</t>
+  </si>
+  <si>
+    <t>jazz brass</t>
+  </si>
+  <si>
+    <t>jazz fusion</t>
+  </si>
+  <si>
+    <t>jazz rap</t>
+  </si>
+  <si>
+    <t>jazz rock</t>
+  </si>
+  <si>
+    <t>jazz saxophone</t>
+  </si>
+  <si>
+    <t>jazz vibraphone</t>
+  </si>
+  <si>
+    <t>jazz violin</t>
+  </si>
+  <si>
+    <t>kansas hip hop</t>
+  </si>
+  <si>
+    <t>kizomba</t>
+  </si>
+  <si>
+    <t>la indie</t>
+  </si>
+  <si>
+    <t>latin funk</t>
+  </si>
+  <si>
+    <t>latin hip hop</t>
+  </si>
+  <si>
+    <t>latvian hip hop</t>
+  </si>
+  <si>
+    <t>lds</t>
+  </si>
+  <si>
+    <t>library music</t>
+  </si>
+  <si>
+    <t>lounge</t>
+  </si>
+  <si>
+    <t>melodic hard rock</t>
+  </si>
+  <si>
+    <t>milwaukee hip hop</t>
+  </si>
+  <si>
+    <t>modern country rock</t>
+  </si>
+  <si>
+    <t>modern power pop</t>
+  </si>
+  <si>
+    <t>modern southern rock</t>
+  </si>
+  <si>
+    <t>musica infantil</t>
+  </si>
+  <si>
+    <t>new americana</t>
+  </si>
+  <si>
+    <t>new french touch</t>
+  </si>
+  <si>
+    <t>new jack smooth</t>
+  </si>
+  <si>
+    <t>oi</t>
+  </si>
+  <si>
+    <t>old school hip hop</t>
+  </si>
+  <si>
+    <t>otacore</t>
+  </si>
+  <si>
+    <t>p funk</t>
+  </si>
+  <si>
+    <t>piano cover</t>
+  </si>
+  <si>
+    <t>polish alternative rap</t>
+  </si>
+  <si>
+    <t>pop soul</t>
+  </si>
+  <si>
+    <t>progressive psytrance</t>
+  </si>
+  <si>
+    <t>progressive rock</t>
+  </si>
+  <si>
+    <t>psychedelic folk</t>
+  </si>
+  <si>
+    <t>r&amp;b en espanol</t>
+  </si>
+  <si>
+    <t>rap kreyol</t>
+  </si>
+  <si>
+    <t>rock drums</t>
+  </si>
+  <si>
+    <t>sad rap</t>
+  </si>
+  <si>
+    <t>san diego rap</t>
+  </si>
+  <si>
+    <t>scorecore</t>
+  </si>
+  <si>
+    <t>screamo</t>
+  </si>
+  <si>
+    <t>shush</t>
+  </si>
+  <si>
+    <t>ska</t>
+  </si>
+  <si>
+    <t>sleep</t>
+  </si>
+  <si>
+    <t>soca</t>
+  </si>
+  <si>
+    <t>south african jazz</t>
+  </si>
+  <si>
+    <t>southern hip hop</t>
+  </si>
+  <si>
+    <t>spa</t>
+  </si>
+  <si>
+    <t>spiritual hip hop</t>
+  </si>
+  <si>
+    <t>steel guitar</t>
+  </si>
+  <si>
+    <t>sudanese pop</t>
+  </si>
+  <si>
+    <t>swamp blues</t>
+  </si>
+  <si>
+    <t>swedish garage rock</t>
+  </si>
+  <si>
+    <t>swedish indie rock</t>
+  </si>
+  <si>
+    <t>talent show</t>
+  </si>
+  <si>
+    <t>tejano</t>
+  </si>
+  <si>
+    <t>traditional rockabilly</t>
+  </si>
+  <si>
+    <t>tribal house</t>
+  </si>
+  <si>
+    <t>tropical house</t>
+  </si>
+  <si>
+    <t>turntablism</t>
+  </si>
+  <si>
+    <t>uk contemporary r&amp;b</t>
+  </si>
+  <si>
+    <t>upstate ny rap</t>
+  </si>
+  <si>
+    <t>v-pop</t>
+  </si>
+  <si>
+    <t>vapor pop</t>
+  </si>
+  <si>
+    <t>vintage french electronic</t>
+  </si>
+  <si>
+    <t>vintage swing</t>
+  </si>
+  <si>
+    <t>viral trap</t>
+  </si>
+  <si>
+    <t>vocal house</t>
+  </si>
+  <si>
+    <t>vocal jazz</t>
+  </si>
+  <si>
+    <t>west coast rap</t>
+  </si>
+  <si>
+    <t>west coast trap</t>
+  </si>
+  <si>
+    <t>wu fam</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/playlist/2GiU50Y6j2oioclfkqlcC4</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Azonto</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Serbische_Brass-Musik</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Bardcore</t>
+  </si>
+  <si>
+    <t>https://remywiki.com/BEMANI</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Bluegrass</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Baltimore_club</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Boston_Hardcore</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/playlist/78MPGFVq0C4yrfvgxZKngM</t>
+  </si>
+  <si>
+    <t>https://www.last.fm/tag/cantautor</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Champeta</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Corrosion_of_Conformity</t>
+  </si>
+  <si>
+    <t>https://www.nodepression.com/what-is-cosmic-american-music-and-a-list-of-examples/</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Cumbia</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/playlist/0J8pO9hK5KnAFWaLE3oTfK</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Elephant_6</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Enka</t>
+  </si>
+  <si>
+    <t>https://festivalpeak.com/what-is-escape-room-and-why-is-it-one-of-my-top-genres-on-spotify-a886372f003f</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Gabber</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/playlist/3pENYVTMuevP3CLjzQkDpQ</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Hyphy</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Kizomba</t>
+  </si>
+  <si>
+    <t>https://www.pinterest.ch/klauspiotrowski/lds-music/</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/playlist/7m1pFx600mZCOuIsOoEIZW</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=aaFPFqJ6QBw</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Oi!</t>
+  </si>
+  <si>
+    <t>https://www.musicianwave.com/what-is-otacore-music-a-clear-explanation/</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/playlist/1v75VUwKR28oOd6Lf3C6JD</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Screamo</t>
+  </si>
+  <si>
+    <t>https://shushmusic.com/</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Ska</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Soca_(Musikrichtung)</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Tejano_music</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Turntablism</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Wu-Tang_Clan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">classical - mostly instrumental </t>
   </si>
 </sst>
 </file>
@@ -2057,10 +2723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{015A9F8D-F621-4F22-B236-0DC5469AB275}">
-  <dimension ref="A1:C485"/>
+  <dimension ref="A1:C672"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A588" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B648" sqref="B648"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2077,7 +2743,7 @@
         <v>484</v>
       </c>
       <c r="C1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2325,7 +2991,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
       <c r="C32" t="s">
         <v>492</v>
@@ -2589,7 +3255,7 @@
         <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>488</v>
+        <v>160</v>
       </c>
       <c r="C62" t="s">
         <v>497</v>
@@ -2600,7 +3266,7 @@
         <v>60</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
       <c r="C63" s="3"/>
     </row>
@@ -3036,7 +3702,7 @@
         <v>112</v>
       </c>
       <c r="B115" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
       <c r="C115" t="s">
         <v>505</v>
@@ -3221,7 +3887,7 @@
         <v>134</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
@@ -3293,7 +3959,7 @@
         <v>143</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
@@ -3576,7 +4242,7 @@
         <v>178</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
@@ -3587,7 +4253,7 @@
         <v>486</v>
       </c>
       <c r="C182" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
@@ -3611,7 +4277,7 @@
         <v>182</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
@@ -3619,7 +4285,7 @@
         <v>183</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
@@ -3651,7 +4317,7 @@
         <v>187</v>
       </c>
       <c r="B190" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
@@ -3675,7 +4341,7 @@
         <v>190</v>
       </c>
       <c r="B193" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
@@ -3694,7 +4360,7 @@
         <v>485</v>
       </c>
       <c r="C195" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
@@ -3705,7 +4371,7 @@
         <v>258</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
@@ -3748,7 +4414,7 @@
         <v>486</v>
       </c>
       <c r="C201" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
@@ -3772,7 +4438,7 @@
         <v>201</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
@@ -3847,7 +4513,7 @@
         <v>160</v>
       </c>
       <c r="C213" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
@@ -4106,7 +4772,7 @@
         <v>488</v>
       </c>
       <c r="C245" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
@@ -4125,7 +4791,7 @@
         <v>485</v>
       </c>
       <c r="C247" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
@@ -4173,7 +4839,7 @@
         <v>250</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
@@ -4248,7 +4914,7 @@
         <v>166</v>
       </c>
       <c r="C262" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.3">
@@ -4307,7 +4973,7 @@
         <v>166</v>
       </c>
       <c r="C269" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
@@ -4326,7 +4992,7 @@
         <v>486</v>
       </c>
       <c r="C271" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.3">
@@ -4334,7 +5000,7 @@
         <v>269</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
@@ -4398,7 +5064,7 @@
         <v>277</v>
       </c>
       <c r="B280" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
@@ -4470,7 +5136,7 @@
         <v>286</v>
       </c>
       <c r="B289" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.3">
@@ -4569,7 +5235,7 @@
         <v>166</v>
       </c>
       <c r="C301" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
@@ -4665,7 +5331,7 @@
         <v>310</v>
       </c>
       <c r="B313" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.3">
@@ -4684,7 +5350,7 @@
         <v>160</v>
       </c>
       <c r="C315" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.3">
@@ -4708,7 +5374,7 @@
         <v>315</v>
       </c>
       <c r="B318" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.3">
@@ -4767,7 +5433,7 @@
         <v>488</v>
       </c>
       <c r="C325" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.3">
@@ -4850,7 +5516,7 @@
         <v>486</v>
       </c>
       <c r="C335" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.3">
@@ -5021,7 +5687,7 @@
         <v>500</v>
       </c>
       <c r="C356" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.3">
@@ -5064,7 +5730,7 @@
         <v>80</v>
       </c>
       <c r="C361" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.3">
@@ -5155,7 +5821,7 @@
         <v>488</v>
       </c>
       <c r="C372" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.3">
@@ -5190,7 +5856,7 @@
         <v>486</v>
       </c>
       <c r="C376" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.3">
@@ -5209,7 +5875,7 @@
         <v>160</v>
       </c>
       <c r="C378" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.3">
@@ -5260,7 +5926,7 @@
         <v>166</v>
       </c>
       <c r="C384" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.3">
@@ -5343,7 +6009,7 @@
         <v>500</v>
       </c>
       <c r="C394" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.3">
@@ -5530,7 +6196,7 @@
         <v>160</v>
       </c>
       <c r="C417" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.3">
@@ -5602,7 +6268,7 @@
         <v>423</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.3">
@@ -5621,7 +6287,7 @@
         <v>486</v>
       </c>
       <c r="C428" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.3">
@@ -5632,7 +6298,7 @@
         <v>160</v>
       </c>
       <c r="C429" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.3">
@@ -5675,7 +6341,7 @@
         <v>166</v>
       </c>
       <c r="C434" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.3">
@@ -5686,7 +6352,7 @@
         <v>488</v>
       </c>
       <c r="C435" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.3">
@@ -5761,7 +6427,7 @@
         <v>166</v>
       </c>
       <c r="C444" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.3">
@@ -5780,7 +6446,7 @@
         <v>500</v>
       </c>
       <c r="C446" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.3">
@@ -5852,10 +6518,10 @@
         <v>452</v>
       </c>
       <c r="B455" t="s">
-        <v>509</v>
+        <v>763</v>
       </c>
       <c r="C455" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.3">
@@ -5986,7 +6652,7 @@
         <v>500</v>
       </c>
       <c r="C471" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.3">
@@ -6021,7 +6687,7 @@
         <v>500</v>
       </c>
       <c r="C475" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.3">
@@ -6064,7 +6730,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="481" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
         <v>478</v>
       </c>
@@ -6072,7 +6738,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="482" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A482" t="s">
         <v>479</v>
       </c>
@@ -6080,7 +6746,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="483" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
         <v>480</v>
       </c>
@@ -6088,7 +6754,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="484" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
         <v>481</v>
       </c>
@@ -6096,12 +6762,1613 @@
         <v>486</v>
       </c>
     </row>
-    <row r="485" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
         <v>482</v>
       </c>
       <c r="B485" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A486" t="s">
+        <v>541</v>
+      </c>
+      <c r="B486" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A487" t="s">
+        <v>542</v>
+      </c>
+      <c r="B487" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A488" t="s">
+        <v>543</v>
+      </c>
+      <c r="B488" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A489" t="s">
+        <v>544</v>
+      </c>
+      <c r="B489" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A490" t="s">
+        <v>545</v>
+      </c>
+      <c r="B490" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A491" t="s">
+        <v>546</v>
+      </c>
+      <c r="B491" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A492" t="s">
+        <v>547</v>
+      </c>
+      <c r="B492" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A493" t="s">
+        <v>548</v>
+      </c>
+      <c r="B493" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A494" t="s">
+        <v>549</v>
+      </c>
+      <c r="B494" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="495" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A495" t="s">
+        <v>550</v>
+      </c>
+      <c r="B495" t="s">
+        <v>166</v>
+      </c>
+      <c r="C495" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="496" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A496" t="s">
+        <v>551</v>
+      </c>
+      <c r="B496" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="497" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A497" t="s">
+        <v>552</v>
+      </c>
+      <c r="B497" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="498" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A498" t="s">
+        <v>553</v>
+      </c>
+      <c r="B498" t="s">
+        <v>488</v>
+      </c>
+      <c r="C498" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A499" t="s">
+        <v>554</v>
+      </c>
+      <c r="B499" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A500" t="s">
+        <v>555</v>
+      </c>
+      <c r="B500" t="s">
+        <v>160</v>
+      </c>
+      <c r="C500" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="501" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A501" t="s">
+        <v>556</v>
+      </c>
+      <c r="B501" t="s">
+        <v>160</v>
+      </c>
+      <c r="C501" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="502" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A502" t="s">
+        <v>557</v>
+      </c>
+      <c r="B502" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="503" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A503" t="s">
+        <v>558</v>
+      </c>
+      <c r="B503" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="504" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A504" t="s">
+        <v>559</v>
+      </c>
+      <c r="B504" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="505" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A505" t="s">
+        <v>560</v>
+      </c>
+      <c r="B505" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A506" t="s">
+        <v>561</v>
+      </c>
+      <c r="B506" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="507" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A507" t="s">
+        <v>562</v>
+      </c>
+      <c r="B507" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="508" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A508" t="s">
+        <v>563</v>
+      </c>
+      <c r="B508" t="s">
+        <v>166</v>
+      </c>
+      <c r="C508" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="509" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A509" t="s">
+        <v>564</v>
+      </c>
+      <c r="B509" t="s">
+        <v>160</v>
+      </c>
+      <c r="C509" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="510" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A510" t="s">
+        <v>565</v>
+      </c>
+      <c r="B510" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="511" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A511" t="s">
+        <v>566</v>
+      </c>
+      <c r="B511" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="512" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A512" t="s">
+        <v>567</v>
+      </c>
+      <c r="B512" t="s">
+        <v>500</v>
+      </c>
+      <c r="C512" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="513" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A513" t="s">
+        <v>568</v>
+      </c>
+      <c r="B513" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="514" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A514" t="s">
+        <v>569</v>
+      </c>
+      <c r="B514" t="s">
+        <v>486</v>
+      </c>
+      <c r="C514" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="515" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A515" t="s">
+        <v>570</v>
+      </c>
+      <c r="B515" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="516" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A516" t="s">
+        <v>571</v>
+      </c>
+      <c r="B516" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="517" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A517" t="s">
+        <v>572</v>
+      </c>
+      <c r="B517" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="518" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A518" t="s">
+        <v>573</v>
+      </c>
+      <c r="B518" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="519" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A519" t="s">
+        <v>574</v>
+      </c>
+      <c r="B519" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="520" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A520" t="s">
+        <v>575</v>
+      </c>
+      <c r="B520" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="521" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A521" t="s">
+        <v>576</v>
+      </c>
+      <c r="B521" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="522" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A522" t="s">
+        <v>577</v>
+      </c>
+      <c r="B522" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="523" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A523" t="s">
+        <v>578</v>
+      </c>
+      <c r="B523" t="s">
+        <v>166</v>
+      </c>
+      <c r="C523" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="524" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A524" t="s">
+        <v>579</v>
+      </c>
+      <c r="B524" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="525" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A525" t="s">
+        <v>580</v>
+      </c>
+      <c r="B525" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="526" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A526" t="s">
+        <v>581</v>
+      </c>
+      <c r="B526" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="527" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A527" t="s">
+        <v>582</v>
+      </c>
+      <c r="B527" t="s">
+        <v>363</v>
+      </c>
+      <c r="C527" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="528" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A528" t="s">
+        <v>583</v>
+      </c>
+      <c r="B528" t="s">
+        <v>363</v>
+      </c>
+      <c r="C528" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="529" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A529" t="s">
+        <v>584</v>
+      </c>
+      <c r="B529" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="530" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A530" t="s">
+        <v>585</v>
+      </c>
+      <c r="B530" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="531" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A531" t="s">
+        <v>586</v>
+      </c>
+      <c r="B531" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="532" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A532" t="s">
+        <v>587</v>
+      </c>
+      <c r="B532" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="533" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A533" t="s">
+        <v>588</v>
+      </c>
+      <c r="B533" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="534" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A534" t="s">
+        <v>589</v>
+      </c>
+      <c r="B534" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="535" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A535" t="s">
+        <v>590</v>
+      </c>
+      <c r="B535" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="536" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A536" t="s">
+        <v>591</v>
+      </c>
+      <c r="B536" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="537" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A537" t="s">
+        <v>592</v>
+      </c>
+      <c r="B537" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="538" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A538" t="s">
+        <v>593</v>
+      </c>
+      <c r="B538" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="539" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A539" t="s">
+        <v>594</v>
+      </c>
+      <c r="B539" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="540" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A540" t="s">
+        <v>595</v>
+      </c>
+      <c r="B540" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="541" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A541" t="s">
+        <v>596</v>
+      </c>
+      <c r="B541" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="542" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A542" t="s">
+        <v>597</v>
+      </c>
+      <c r="B542" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="543" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A543" t="s">
+        <v>598</v>
+      </c>
+      <c r="B543" t="s">
+        <v>486</v>
+      </c>
+      <c r="C543" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="544" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A544" t="s">
+        <v>599</v>
+      </c>
+      <c r="B544" t="s">
+        <v>80</v>
+      </c>
+      <c r="C544" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="545" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A545" t="s">
+        <v>600</v>
+      </c>
+      <c r="B545" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="546" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A546" t="s">
+        <v>601</v>
+      </c>
+      <c r="B546" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="547" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A547" t="s">
+        <v>602</v>
+      </c>
+      <c r="B547" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="548" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A548" t="s">
+        <v>603</v>
+      </c>
+      <c r="B548" t="s">
+        <v>363</v>
+      </c>
+      <c r="C548" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="549" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A549" t="s">
+        <v>604</v>
+      </c>
+      <c r="B549" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="550" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A550" t="s">
+        <v>605</v>
+      </c>
+      <c r="B550" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="551" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A551" t="s">
+        <v>606</v>
+      </c>
+      <c r="B551" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="552" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A552" t="s">
+        <v>607</v>
+      </c>
+      <c r="B552" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="553" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A553" t="s">
+        <v>608</v>
+      </c>
+      <c r="B553" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="554" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A554" t="s">
+        <v>609</v>
+      </c>
+      <c r="B554" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="555" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A555" t="s">
+        <v>610</v>
+      </c>
+      <c r="B555" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="556" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A556" t="s">
+        <v>611</v>
+      </c>
+      <c r="B556" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="557" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A557" t="s">
+        <v>612</v>
+      </c>
+      <c r="B557" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="558" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A558" t="s">
+        <v>613</v>
+      </c>
+      <c r="B558" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="559" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A559" t="s">
+        <v>614</v>
+      </c>
+      <c r="B559" t="s">
+        <v>80</v>
+      </c>
+      <c r="C559" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="560" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A560" t="s">
+        <v>615</v>
+      </c>
+      <c r="B560" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="561" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A561" t="s">
+        <v>616</v>
+      </c>
+      <c r="B561" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="562" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A562" t="s">
+        <v>617</v>
+      </c>
+      <c r="B562" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="563" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A563" t="s">
+        <v>618</v>
+      </c>
+      <c r="B563" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="564" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A564" t="s">
+        <v>619</v>
+      </c>
+      <c r="B564" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="565" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A565" t="s">
+        <v>620</v>
+      </c>
+      <c r="B565" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="566" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A566" t="s">
+        <v>621</v>
+      </c>
+      <c r="B566" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="567" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A567" t="s">
+        <v>622</v>
+      </c>
+      <c r="B567" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="568" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A568" t="s">
+        <v>623</v>
+      </c>
+      <c r="B568" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="569" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A569" t="s">
+        <v>624</v>
+      </c>
+      <c r="B569" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="570" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A570" t="s">
+        <v>625</v>
+      </c>
+      <c r="B570" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="571" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A571" t="s">
+        <v>626</v>
+      </c>
+      <c r="B571" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="572" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A572" t="s">
+        <v>627</v>
+      </c>
+      <c r="B572" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="573" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A573" t="s">
+        <v>628</v>
+      </c>
+      <c r="B573" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="574" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A574" t="s">
+        <v>629</v>
+      </c>
+      <c r="B574" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="575" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A575" t="s">
+        <v>630</v>
+      </c>
+      <c r="B575" t="s">
+        <v>8</v>
+      </c>
+      <c r="C575" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="576" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A576" t="s">
+        <v>631</v>
+      </c>
+      <c r="B576" t="s">
+        <v>160</v>
+      </c>
+      <c r="C576" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="577" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A577" t="s">
+        <v>632</v>
+      </c>
+      <c r="B577" t="s">
+        <v>763</v>
+      </c>
+      <c r="C577" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="578" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A578" t="s">
+        <v>633</v>
+      </c>
+      <c r="B578" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="579" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A579" t="s">
+        <v>634</v>
+      </c>
+      <c r="B579" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="580" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A580" t="s">
+        <v>635</v>
+      </c>
+      <c r="B580" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="581" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A581" t="s">
+        <v>636</v>
+      </c>
+      <c r="B581" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="582" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A582" t="s">
+        <v>637</v>
+      </c>
+      <c r="B582" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="583" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A583" t="s">
+        <v>638</v>
+      </c>
+      <c r="B583" t="s">
+        <v>488</v>
+      </c>
+      <c r="C583" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="584" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A584" t="s">
+        <v>639</v>
+      </c>
+      <c r="B584" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="585" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A585" t="s">
+        <v>640</v>
+      </c>
+      <c r="B585" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="586" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A586" t="s">
+        <v>641</v>
+      </c>
+      <c r="B586" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="587" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A587" t="s">
+        <v>642</v>
+      </c>
+      <c r="B587" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="588" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A588" t="s">
+        <v>643</v>
+      </c>
+      <c r="B588" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="589" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A589" t="s">
+        <v>644</v>
+      </c>
+      <c r="B589" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="590" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A590" t="s">
+        <v>645</v>
+      </c>
+      <c r="B590" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="591" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A591" t="s">
+        <v>646</v>
+      </c>
+      <c r="B591" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="592" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A592" t="s">
+        <v>647</v>
+      </c>
+      <c r="B592" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="593" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A593" t="s">
+        <v>648</v>
+      </c>
+      <c r="B593" t="s">
+        <v>166</v>
+      </c>
+      <c r="C593" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="594" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A594" t="s">
+        <v>649</v>
+      </c>
+      <c r="B594" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="595" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A595" t="s">
+        <v>650</v>
+      </c>
+      <c r="B595" t="s">
+        <v>500</v>
+      </c>
+      <c r="C595" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="596" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A596" t="s">
+        <v>651</v>
+      </c>
+      <c r="B596" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="597" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A597" t="s">
+        <v>652</v>
+      </c>
+      <c r="B597" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="598" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A598" t="s">
+        <v>653</v>
+      </c>
+      <c r="B598" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="599" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A599" t="s">
+        <v>654</v>
+      </c>
+      <c r="B599" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="600" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A600" t="s">
+        <v>655</v>
+      </c>
+      <c r="B600" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="601" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A601" t="s">
+        <v>656</v>
+      </c>
+      <c r="B601" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="602" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A602" t="s">
+        <v>657</v>
+      </c>
+      <c r="B602" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="603" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A603" t="s">
+        <v>658</v>
+      </c>
+      <c r="B603" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="604" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A604" t="s">
+        <v>659</v>
+      </c>
+      <c r="B604" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="605" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A605" t="s">
+        <v>660</v>
+      </c>
+      <c r="B605" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="606" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A606" t="s">
+        <v>661</v>
+      </c>
+      <c r="B606" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="607" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A607" t="s">
+        <v>662</v>
+      </c>
+      <c r="B607" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="608" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A608" t="s">
+        <v>663</v>
+      </c>
+      <c r="B608" t="s">
+        <v>160</v>
+      </c>
+      <c r="C608" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="609" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A609" t="s">
+        <v>664</v>
+      </c>
+      <c r="B609" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="610" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A610" t="s">
+        <v>665</v>
+      </c>
+      <c r="B610" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="611" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A611" t="s">
+        <v>666</v>
+      </c>
+      <c r="B611" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="612" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A612" t="s">
+        <v>667</v>
+      </c>
+      <c r="B612" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="613" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A613" t="s">
+        <v>668</v>
+      </c>
+      <c r="B613" t="s">
+        <v>160</v>
+      </c>
+      <c r="C613" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="614" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A614" t="s">
+        <v>669</v>
+      </c>
+      <c r="B614" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="615" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A615" t="s">
+        <v>670</v>
+      </c>
+      <c r="B615" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="616" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A616" t="s">
+        <v>671</v>
+      </c>
+      <c r="B616" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="617" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A617" t="s">
+        <v>672</v>
+      </c>
+      <c r="B617" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="618" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A618" t="s">
+        <v>673</v>
+      </c>
+      <c r="B618" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="619" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A619" t="s">
+        <v>674</v>
+      </c>
+      <c r="B619" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="620" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A620" t="s">
+        <v>675</v>
+      </c>
+      <c r="B620" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="621" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A621" t="s">
+        <v>676</v>
+      </c>
+      <c r="B621" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="622" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A622" t="s">
+        <v>677</v>
+      </c>
+      <c r="B622" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="623" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A623" t="s">
+        <v>678</v>
+      </c>
+      <c r="B623" t="s">
+        <v>500</v>
+      </c>
+      <c r="C623" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="624" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A624" t="s">
+        <v>679</v>
+      </c>
+      <c r="B624" t="s">
+        <v>500</v>
+      </c>
+      <c r="C624" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="625" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A625" t="s">
+        <v>680</v>
+      </c>
+      <c r="B625" t="s">
+        <v>486</v>
+      </c>
+      <c r="C625" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="626" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A626" t="s">
+        <v>681</v>
+      </c>
+      <c r="B626" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="627" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A627" t="s">
+        <v>682</v>
+      </c>
+      <c r="B627" t="s">
+        <v>166</v>
+      </c>
+      <c r="C627" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="628" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A628" t="s">
+        <v>683</v>
+      </c>
+      <c r="B628" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="629" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A629" t="s">
+        <v>684</v>
+      </c>
+      <c r="B629" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="630" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A630" t="s">
+        <v>685</v>
+      </c>
+      <c r="B630" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="631" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A631" t="s">
+        <v>686</v>
+      </c>
+      <c r="B631" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="632" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A632" t="s">
+        <v>687</v>
+      </c>
+      <c r="B632" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="633" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A633" t="s">
+        <v>688</v>
+      </c>
+      <c r="B633" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="634" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A634" t="s">
+        <v>689</v>
+      </c>
+      <c r="B634" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="635" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A635" t="s">
+        <v>690</v>
+      </c>
+      <c r="B635" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="636" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A636" t="s">
+        <v>691</v>
+      </c>
+      <c r="B636" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="637" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A637" t="s">
+        <v>692</v>
+      </c>
+      <c r="B637" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="638" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A638" t="s">
+        <v>693</v>
+      </c>
+      <c r="B638" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="639" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A639" t="s">
+        <v>694</v>
+      </c>
+      <c r="B639" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="640" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A640" t="s">
+        <v>695</v>
+      </c>
+      <c r="B640" t="s">
+        <v>763</v>
+      </c>
+      <c r="C640" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="641" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A641" t="s">
+        <v>696</v>
+      </c>
+      <c r="B641" t="s">
+        <v>486</v>
+      </c>
+      <c r="C641" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="642" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A642" t="s">
+        <v>697</v>
+      </c>
+      <c r="B642" t="s">
+        <v>488</v>
+      </c>
+      <c r="C642" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="643" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A643" t="s">
+        <v>698</v>
+      </c>
+      <c r="B643" t="s">
+        <v>258</v>
+      </c>
+      <c r="C643" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="644" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A644" t="s">
+        <v>699</v>
+      </c>
+      <c r="B644" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="645" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A645" t="s">
+        <v>700</v>
+      </c>
+      <c r="B645" t="s">
+        <v>160</v>
+      </c>
+      <c r="C645" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="646" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A646" t="s">
+        <v>701</v>
+      </c>
+      <c r="B646" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="647" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A647" t="s">
+        <v>702</v>
+      </c>
+      <c r="B647" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="648" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A648" t="s">
+        <v>703</v>
+      </c>
+      <c r="B648" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="649" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A649" t="s">
+        <v>704</v>
+      </c>
+      <c r="B649" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="650" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A650" t="s">
+        <v>705</v>
+      </c>
+      <c r="B650" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="651" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A651" t="s">
+        <v>706</v>
+      </c>
+      <c r="B651" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="652" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A652" t="s">
+        <v>707</v>
+      </c>
+      <c r="B652" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="653" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A653" t="s">
+        <v>708</v>
+      </c>
+      <c r="B653" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="654" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A654" t="s">
+        <v>709</v>
+      </c>
+      <c r="B654" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="655" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A655" t="s">
+        <v>710</v>
+      </c>
+      <c r="B655" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="656" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A656" t="s">
+        <v>711</v>
+      </c>
+      <c r="B656" t="s">
+        <v>363</v>
+      </c>
+      <c r="C656" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="657" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A657" t="s">
+        <v>712</v>
+      </c>
+      <c r="B657" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="658" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A658" t="s">
+        <v>713</v>
+      </c>
+      <c r="B658" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="659" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A659" t="s">
+        <v>714</v>
+      </c>
+      <c r="B659" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="660" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A660" t="s">
+        <v>715</v>
+      </c>
+      <c r="B660" t="s">
+        <v>500</v>
+      </c>
+      <c r="C660" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="661" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A661" t="s">
+        <v>716</v>
+      </c>
+      <c r="B661" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="662" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A662" t="s">
+        <v>717</v>
+      </c>
+      <c r="B662" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="663" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A663" t="s">
+        <v>718</v>
+      </c>
+      <c r="B663" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="664" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A664" t="s">
+        <v>719</v>
+      </c>
+      <c r="B664" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="665" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A665" t="s">
+        <v>720</v>
+      </c>
+      <c r="B665" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="666" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A666" t="s">
+        <v>721</v>
+      </c>
+      <c r="B666" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="667" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A667" t="s">
+        <v>722</v>
+      </c>
+      <c r="B667" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="668" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A668" t="s">
+        <v>723</v>
+      </c>
+      <c r="B668" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="669" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A669" t="s">
+        <v>724</v>
+      </c>
+      <c r="B669" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="670" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A670" t="s">
+        <v>725</v>
+      </c>
+      <c r="B670" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="671" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A671" t="s">
+        <v>726</v>
+      </c>
+      <c r="B671" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="672" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A672" t="s">
+        <v>727</v>
+      </c>
+      <c r="B672" t="s">
+        <v>500</v>
+      </c>
+      <c r="C672" t="s">
+        <v>762</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some new genres added (also including the last fm API)
</commit_message>
<xml_diff>
--- a/unique_genres.xlsx
+++ b/unique_genres.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Documents\Uni\3. Sem\DS Projekt\Code_and_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F6BFAC-0ECC-4776-9CD9-A3C594AA67B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8923B2-0FC7-4F7A-82B2-CF358FD17958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$B$1:$B$485</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$B$1:$B$672</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="806">
   <si>
     <t>adult standards</t>
   </si>
@@ -1486,9 +1486,6 @@
     <t>rock</t>
   </si>
   <si>
-    <t>classic</t>
-  </si>
-  <si>
     <t>dance</t>
   </si>
   <si>
@@ -2314,7 +2311,136 @@
     <t>https://de.wikipedia.org/wiki/Wu-Tang_Clan</t>
   </si>
   <si>
-    <t xml:space="preserve">classical - mostly instrumental </t>
+    <t>!!!</t>
+  </si>
+  <si>
+    <t>r and b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">party </t>
+  </si>
+  <si>
+    <t>doo wop</t>
+  </si>
+  <si>
+    <t>instrumental</t>
+  </si>
+  <si>
+    <t>jazz</t>
+  </si>
+  <si>
+    <t>rock n roll</t>
+  </si>
+  <si>
+    <t>swing</t>
+  </si>
+  <si>
+    <t>surf</t>
+  </si>
+  <si>
+    <t>heavy metal</t>
+  </si>
+  <si>
+    <t>latin rock</t>
+  </si>
+  <si>
+    <t>electronic</t>
+  </si>
+  <si>
+    <t>country-rock</t>
+  </si>
+  <si>
+    <t>popular</t>
+  </si>
+  <si>
+    <t>space</t>
+  </si>
+  <si>
+    <t>love</t>
+  </si>
+  <si>
+    <t>looove</t>
+  </si>
+  <si>
+    <t>west coast</t>
+  </si>
+  <si>
+    <t>funk tag</t>
+  </si>
+  <si>
+    <t>goth</t>
+  </si>
+  <si>
+    <t>hip-hop</t>
+  </si>
+  <si>
+    <t>alternative</t>
+  </si>
+  <si>
+    <t>trance</t>
+  </si>
+  <si>
+    <t>hair metal</t>
+  </si>
+  <si>
+    <t>gangsta rap</t>
+  </si>
+  <si>
+    <t>trip-hop</t>
+  </si>
+  <si>
+    <t>punk rock</t>
+  </si>
+  <si>
+    <t>pop music tag</t>
+  </si>
+  <si>
+    <t>progressive metal</t>
+  </si>
+  <si>
+    <t>contemporary rnb</t>
+  </si>
+  <si>
+    <t>indie</t>
+  </si>
+  <si>
+    <t>reggaeton</t>
+  </si>
+  <si>
+    <t>christmas</t>
+  </si>
+  <si>
+    <t>alternative rnb</t>
+  </si>
+  <si>
+    <t>piano rock</t>
+  </si>
+  <si>
+    <t>trash metal</t>
+  </si>
+  <si>
+    <t>metal</t>
+  </si>
+  <si>
+    <t>dubstep</t>
+  </si>
+  <si>
+    <t>new rave</t>
+  </si>
+  <si>
+    <t>hiphop</t>
+  </si>
+  <si>
+    <t>east coast hip-hop</t>
+  </si>
+  <si>
+    <t>trap rap</t>
+  </si>
+  <si>
+    <t>kpop</t>
+  </si>
+  <si>
+    <t>zumba</t>
   </si>
 </sst>
 </file>
@@ -2723,10 +2849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{015A9F8D-F621-4F22-B236-0DC5469AB275}">
-  <dimension ref="A1:C672"/>
+  <dimension ref="A1:H719"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A588" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B648" sqref="B648"/>
+    <sheetView tabSelected="1" topLeftCell="A686" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B701" sqref="B701"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2735,7 +2861,7 @@
     <col min="2" max="2" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>483</v>
       </c>
@@ -2743,10 +2869,10 @@
         <v>484</v>
       </c>
       <c r="C1" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2754,7 +2880,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2762,7 +2888,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2770,7 +2896,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2778,7 +2904,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2786,7 +2912,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2794,7 +2920,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2802,7 +2928,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -2810,15 +2936,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>762</v>
+      </c>
+      <c r="H10" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2826,7 +2958,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2834,7 +2966,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2842,7 +2974,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2850,7 +2982,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2858,7 +2990,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2991,10 +3123,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
       <c r="C32" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -3053,7 +3185,7 @@
         <v>166</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -3120,7 +3252,7 @@
         <v>166</v>
       </c>
       <c r="C47" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -3139,7 +3271,7 @@
         <v>485</v>
       </c>
       <c r="C49" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -3158,7 +3290,7 @@
         <v>166</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -3193,7 +3325,7 @@
         <v>166</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -3236,7 +3368,7 @@
         <v>166</v>
       </c>
       <c r="C60" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -3247,7 +3379,7 @@
         <v>485</v>
       </c>
       <c r="C61" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -3258,7 +3390,7 @@
         <v>160</v>
       </c>
       <c r="C62" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -3266,7 +3398,7 @@
         <v>60</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
       <c r="C63" s="3"/>
     </row>
@@ -3291,8 +3423,8 @@
       <c r="A66" t="s">
         <v>63</v>
       </c>
-      <c r="B66" t="s">
-        <v>487</v>
+      <c r="B66" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -3308,7 +3440,7 @@
         <v>65</v>
       </c>
       <c r="B68" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -3316,7 +3448,7 @@
         <v>66</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -3335,15 +3467,15 @@
         <v>166</v>
       </c>
       <c r="C71" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>69</v>
       </c>
-      <c r="B72" t="s">
-        <v>487</v>
+      <c r="B72" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -3366,8 +3498,8 @@
       <c r="A75" t="s">
         <v>72</v>
       </c>
-      <c r="B75" t="s">
-        <v>487</v>
+      <c r="B75" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -3378,7 +3510,7 @@
         <v>8</v>
       </c>
       <c r="C76" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -3394,7 +3526,7 @@
         <v>75</v>
       </c>
       <c r="B78" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -3402,7 +3534,7 @@
         <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -3541,7 +3673,7 @@
         <v>80</v>
       </c>
       <c r="C96" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -3549,7 +3681,7 @@
         <v>94</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
@@ -3612,8 +3744,8 @@
       <c r="A105" t="s">
         <v>102</v>
       </c>
-      <c r="B105" t="s">
-        <v>487</v>
+      <c r="B105" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -3640,7 +3772,7 @@
         <v>486</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
@@ -3663,8 +3795,8 @@
       <c r="A111" t="s">
         <v>108</v>
       </c>
-      <c r="B111" t="s">
-        <v>487</v>
+      <c r="B111" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
@@ -3675,7 +3807,7 @@
         <v>160</v>
       </c>
       <c r="C112" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -3694,7 +3826,7 @@
         <v>166</v>
       </c>
       <c r="C114" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -3702,10 +3834,10 @@
         <v>112</v>
       </c>
       <c r="B115" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
       <c r="C115" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -3721,7 +3853,7 @@
         <v>114</v>
       </c>
       <c r="B117" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -3737,7 +3869,7 @@
         <v>116</v>
       </c>
       <c r="B119" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
@@ -3777,7 +3909,7 @@
         <v>121</v>
       </c>
       <c r="B124" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -3809,10 +3941,10 @@
         <v>125</v>
       </c>
       <c r="B128" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C128" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
@@ -3823,15 +3955,15 @@
         <v>485</v>
       </c>
       <c r="C129" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>127</v>
       </c>
-      <c r="B130" t="s">
-        <v>487</v>
+      <c r="B130" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -3847,7 +3979,7 @@
         <v>129</v>
       </c>
       <c r="B132" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
@@ -3887,7 +4019,7 @@
         <v>134</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
@@ -3935,7 +4067,7 @@
         <v>140</v>
       </c>
       <c r="B143" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
@@ -3943,7 +4075,7 @@
         <v>141</v>
       </c>
       <c r="B144" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
@@ -3959,7 +4091,7 @@
         <v>143</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
@@ -3982,8 +4114,8 @@
       <c r="A149" t="s">
         <v>146</v>
       </c>
-      <c r="B149" t="s">
-        <v>487</v>
+      <c r="B149" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
@@ -4087,7 +4219,7 @@
         <v>159</v>
       </c>
       <c r="B162" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -4135,7 +4267,7 @@
         <v>165</v>
       </c>
       <c r="B168" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
@@ -4162,7 +4294,7 @@
         <v>160</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
@@ -4226,7 +4358,7 @@
         <v>176</v>
       </c>
       <c r="B179" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
@@ -4242,7 +4374,7 @@
         <v>178</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
@@ -4253,7 +4385,7 @@
         <v>486</v>
       </c>
       <c r="C182" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
@@ -4277,7 +4409,7 @@
         <v>182</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
@@ -4285,7 +4417,7 @@
         <v>183</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
@@ -4301,7 +4433,7 @@
         <v>185</v>
       </c>
       <c r="B188" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
@@ -4317,7 +4449,7 @@
         <v>187</v>
       </c>
       <c r="B190" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
@@ -4341,7 +4473,7 @@
         <v>190</v>
       </c>
       <c r="B193" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
@@ -4360,7 +4492,7 @@
         <v>485</v>
       </c>
       <c r="C195" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
@@ -4371,7 +4503,7 @@
         <v>258</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
@@ -4414,7 +4546,7 @@
         <v>486</v>
       </c>
       <c r="C201" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
@@ -4438,7 +4570,7 @@
         <v>201</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
@@ -4470,7 +4602,7 @@
         <v>205</v>
       </c>
       <c r="B208" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
@@ -4502,7 +4634,7 @@
         <v>209</v>
       </c>
       <c r="B212" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
@@ -4513,7 +4645,7 @@
         <v>160</v>
       </c>
       <c r="C213" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
@@ -4521,7 +4653,7 @@
         <v>211</v>
       </c>
       <c r="B214" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
@@ -4545,7 +4677,7 @@
         <v>214</v>
       </c>
       <c r="B217" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
@@ -4553,7 +4685,7 @@
         <v>215</v>
       </c>
       <c r="B218" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
@@ -4609,7 +4741,7 @@
         <v>222</v>
       </c>
       <c r="B225" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
@@ -4633,7 +4765,7 @@
         <v>225</v>
       </c>
       <c r="B228" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
@@ -4657,7 +4789,7 @@
         <v>228</v>
       </c>
       <c r="B231" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
@@ -4665,7 +4797,7 @@
         <v>229</v>
       </c>
       <c r="B232" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
@@ -4697,7 +4829,7 @@
         <v>233</v>
       </c>
       <c r="B236" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
@@ -4705,7 +4837,7 @@
         <v>234</v>
       </c>
       <c r="B237" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
@@ -4713,7 +4845,7 @@
         <v>235</v>
       </c>
       <c r="B238" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
@@ -4769,10 +4901,10 @@
         <v>242</v>
       </c>
       <c r="B245" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C245" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
@@ -4791,7 +4923,7 @@
         <v>485</v>
       </c>
       <c r="C247" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
@@ -4807,7 +4939,7 @@
         <v>246</v>
       </c>
       <c r="B249" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
@@ -4831,7 +4963,7 @@
         <v>249</v>
       </c>
       <c r="B252" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
@@ -4839,7 +4971,7 @@
         <v>250</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
@@ -4863,7 +4995,7 @@
         <v>253</v>
       </c>
       <c r="B256" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.3">
@@ -4914,7 +5046,7 @@
         <v>166</v>
       </c>
       <c r="C262" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.3">
@@ -4954,7 +5086,7 @@
         <v>264</v>
       </c>
       <c r="B267" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.3">
@@ -4973,7 +5105,7 @@
         <v>166</v>
       </c>
       <c r="C269" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
@@ -4992,7 +5124,7 @@
         <v>486</v>
       </c>
       <c r="C271" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.3">
@@ -5000,7 +5132,7 @@
         <v>269</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
@@ -5016,7 +5148,7 @@
         <v>271</v>
       </c>
       <c r="B274" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
@@ -5024,7 +5156,7 @@
         <v>272</v>
       </c>
       <c r="B275" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
@@ -5048,7 +5180,7 @@
         <v>275</v>
       </c>
       <c r="B278" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
@@ -5056,7 +5188,7 @@
         <v>276</v>
       </c>
       <c r="B279" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
@@ -5064,7 +5196,7 @@
         <v>277</v>
       </c>
       <c r="B280" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
@@ -5096,7 +5228,7 @@
         <v>281</v>
       </c>
       <c r="B284" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
@@ -5104,7 +5236,7 @@
         <v>282</v>
       </c>
       <c r="B285" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
@@ -5128,7 +5260,7 @@
         <v>285</v>
       </c>
       <c r="B288" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.3">
@@ -5136,7 +5268,7 @@
         <v>286</v>
       </c>
       <c r="B289" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.3">
@@ -5168,7 +5300,7 @@
         <v>290</v>
       </c>
       <c r="B293" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.3">
@@ -5176,7 +5308,7 @@
         <v>291</v>
       </c>
       <c r="B294" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.3">
@@ -5192,7 +5324,7 @@
         <v>293</v>
       </c>
       <c r="B296" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.3">
@@ -5216,7 +5348,7 @@
         <v>296</v>
       </c>
       <c r="B299" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.3">
@@ -5235,7 +5367,7 @@
         <v>166</v>
       </c>
       <c r="C301" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
@@ -5243,7 +5375,7 @@
         <v>299</v>
       </c>
       <c r="B302" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.3">
@@ -5259,7 +5391,7 @@
         <v>301</v>
       </c>
       <c r="B304" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.3">
@@ -5267,7 +5399,7 @@
         <v>302</v>
       </c>
       <c r="B305" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.3">
@@ -5283,7 +5415,7 @@
         <v>304</v>
       </c>
       <c r="B307" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
@@ -5307,7 +5439,7 @@
         <v>307</v>
       </c>
       <c r="B310" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.3">
@@ -5323,7 +5455,7 @@
         <v>309</v>
       </c>
       <c r="B312" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.3">
@@ -5331,7 +5463,7 @@
         <v>310</v>
       </c>
       <c r="B313" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.3">
@@ -5339,7 +5471,7 @@
         <v>311</v>
       </c>
       <c r="B314" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.3">
@@ -5350,7 +5482,7 @@
         <v>160</v>
       </c>
       <c r="C315" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.3">
@@ -5358,7 +5490,7 @@
         <v>313</v>
       </c>
       <c r="B316" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.3">
@@ -5366,7 +5498,7 @@
         <v>314</v>
       </c>
       <c r="B317" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.3">
@@ -5374,7 +5506,7 @@
         <v>315</v>
       </c>
       <c r="B318" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.3">
@@ -5382,7 +5514,7 @@
         <v>316</v>
       </c>
       <c r="B319" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.3">
@@ -5398,7 +5530,7 @@
         <v>318</v>
       </c>
       <c r="B321" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.3">
@@ -5406,7 +5538,7 @@
         <v>319</v>
       </c>
       <c r="B322" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.3">
@@ -5414,7 +5546,7 @@
         <v>320</v>
       </c>
       <c r="B323" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.3">
@@ -5422,7 +5554,7 @@
         <v>321</v>
       </c>
       <c r="B324" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.3">
@@ -5430,10 +5562,10 @@
         <v>322</v>
       </c>
       <c r="B325" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C325" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.3">
@@ -5441,7 +5573,7 @@
         <v>323</v>
       </c>
       <c r="B326" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.3">
@@ -5489,7 +5621,7 @@
         <v>329</v>
       </c>
       <c r="B332" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.3">
@@ -5497,7 +5629,7 @@
         <v>330</v>
       </c>
       <c r="B333" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.3">
@@ -5505,7 +5637,7 @@
         <v>331</v>
       </c>
       <c r="B334" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.3">
@@ -5516,7 +5648,7 @@
         <v>486</v>
       </c>
       <c r="C335" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.3">
@@ -5524,7 +5656,7 @@
         <v>333</v>
       </c>
       <c r="B336" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
@@ -5540,7 +5672,7 @@
         <v>335</v>
       </c>
       <c r="B338" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
@@ -5556,7 +5688,7 @@
         <v>337</v>
       </c>
       <c r="B340" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
@@ -5572,7 +5704,7 @@
         <v>339</v>
       </c>
       <c r="B342" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
@@ -5620,7 +5752,7 @@
         <v>345</v>
       </c>
       <c r="B348" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.3">
@@ -5628,7 +5760,7 @@
         <v>346</v>
       </c>
       <c r="B349" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
@@ -5668,7 +5800,7 @@
         <v>351</v>
       </c>
       <c r="B354" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.3">
@@ -5676,7 +5808,7 @@
         <v>352</v>
       </c>
       <c r="B355" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.3">
@@ -5684,10 +5816,10 @@
         <v>353</v>
       </c>
       <c r="B356" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C356" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.3">
@@ -5695,7 +5827,7 @@
         <v>354</v>
       </c>
       <c r="B357" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.3">
@@ -5730,7 +5862,7 @@
         <v>80</v>
       </c>
       <c r="C361" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.3">
@@ -5738,7 +5870,7 @@
         <v>359</v>
       </c>
       <c r="B362" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.3">
@@ -5746,7 +5878,7 @@
         <v>360</v>
       </c>
       <c r="B363" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.3">
@@ -5754,7 +5886,7 @@
         <v>361</v>
       </c>
       <c r="B364" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.3">
@@ -5802,7 +5934,7 @@
         <v>367</v>
       </c>
       <c r="B370" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.3">
@@ -5818,10 +5950,10 @@
         <v>369</v>
       </c>
       <c r="B372" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C372" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.3">
@@ -5829,7 +5961,7 @@
         <v>370</v>
       </c>
       <c r="B373" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.3">
@@ -5845,7 +5977,7 @@
         <v>372</v>
       </c>
       <c r="B375" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.3">
@@ -5856,7 +5988,7 @@
         <v>486</v>
       </c>
       <c r="C376" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.3">
@@ -5875,7 +6007,7 @@
         <v>160</v>
       </c>
       <c r="C378" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.3">
@@ -5883,7 +6015,7 @@
         <v>376</v>
       </c>
       <c r="B379" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.3">
@@ -5891,7 +6023,7 @@
         <v>377</v>
       </c>
       <c r="B380" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.3">
@@ -5907,7 +6039,7 @@
         <v>379</v>
       </c>
       <c r="B382" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.3">
@@ -5926,7 +6058,7 @@
         <v>166</v>
       </c>
       <c r="C384" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.3">
@@ -5942,7 +6074,7 @@
         <v>383</v>
       </c>
       <c r="B386" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.3">
@@ -5974,7 +6106,7 @@
         <v>387</v>
       </c>
       <c r="B390" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.3">
@@ -6006,10 +6138,10 @@
         <v>391</v>
       </c>
       <c r="B394" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C394" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.3">
@@ -6025,7 +6157,7 @@
         <v>393</v>
       </c>
       <c r="B396" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.3">
@@ -6049,7 +6181,7 @@
         <v>396</v>
       </c>
       <c r="B399" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.3">
@@ -6073,7 +6205,7 @@
         <v>399</v>
       </c>
       <c r="B402" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.3">
@@ -6105,7 +6237,7 @@
         <v>403</v>
       </c>
       <c r="B406" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.3">
@@ -6129,7 +6261,7 @@
         <v>406</v>
       </c>
       <c r="B409" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.3">
@@ -6145,7 +6277,7 @@
         <v>408</v>
       </c>
       <c r="B411" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.3">
@@ -6169,7 +6301,7 @@
         <v>411</v>
       </c>
       <c r="B414" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.3">
@@ -6177,7 +6309,7 @@
         <v>412</v>
       </c>
       <c r="B415" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.3">
@@ -6185,7 +6317,7 @@
         <v>413</v>
       </c>
       <c r="B416" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.3">
@@ -6196,7 +6328,7 @@
         <v>160</v>
       </c>
       <c r="C417" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.3">
@@ -6228,7 +6360,7 @@
         <v>418</v>
       </c>
       <c r="B421" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.3">
@@ -6236,7 +6368,7 @@
         <v>419</v>
       </c>
       <c r="B422" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.3">
@@ -6268,7 +6400,7 @@
         <v>423</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.3">
@@ -6287,7 +6419,7 @@
         <v>486</v>
       </c>
       <c r="C428" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.3">
@@ -6298,7 +6430,7 @@
         <v>160</v>
       </c>
       <c r="C429" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.3">
@@ -6314,7 +6446,7 @@
         <v>428</v>
       </c>
       <c r="B431" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.3">
@@ -6341,7 +6473,7 @@
         <v>166</v>
       </c>
       <c r="C434" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.3">
@@ -6349,10 +6481,10 @@
         <v>432</v>
       </c>
       <c r="B435" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C435" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.3">
@@ -6376,7 +6508,7 @@
         <v>435</v>
       </c>
       <c r="B438" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.3">
@@ -6392,7 +6524,7 @@
         <v>437</v>
       </c>
       <c r="B440" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.3">
@@ -6400,7 +6532,7 @@
         <v>438</v>
       </c>
       <c r="B441" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.3">
@@ -6408,7 +6540,7 @@
         <v>439</v>
       </c>
       <c r="B442" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.3">
@@ -6427,7 +6559,7 @@
         <v>166</v>
       </c>
       <c r="C444" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.3">
@@ -6435,7 +6567,7 @@
         <v>442</v>
       </c>
       <c r="B445" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.3">
@@ -6443,10 +6575,10 @@
         <v>443</v>
       </c>
       <c r="B446" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C446" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.3">
@@ -6470,7 +6602,7 @@
         <v>446</v>
       </c>
       <c r="B449" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.3">
@@ -6486,7 +6618,7 @@
         <v>448</v>
       </c>
       <c r="B451" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.3">
@@ -6494,7 +6626,7 @@
         <v>449</v>
       </c>
       <c r="B452" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.3">
@@ -6510,7 +6642,7 @@
         <v>451</v>
       </c>
       <c r="B454" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.3">
@@ -6518,10 +6650,10 @@
         <v>452</v>
       </c>
       <c r="B455" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
       <c r="C455" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.3">
@@ -6537,7 +6669,7 @@
         <v>454</v>
       </c>
       <c r="B457" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.3">
@@ -6545,7 +6677,7 @@
         <v>455</v>
       </c>
       <c r="B458" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.3">
@@ -6553,7 +6685,7 @@
         <v>456</v>
       </c>
       <c r="B459" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.3">
@@ -6561,7 +6693,7 @@
         <v>457</v>
       </c>
       <c r="B460" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.3">
@@ -6569,7 +6701,7 @@
         <v>458</v>
       </c>
       <c r="B461" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.3">
@@ -6593,7 +6725,7 @@
         <v>461</v>
       </c>
       <c r="B464" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.3">
@@ -6601,7 +6733,7 @@
         <v>462</v>
       </c>
       <c r="B465" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="466" spans="1:3" x14ac:dyDescent="0.3">
@@ -6609,7 +6741,7 @@
         <v>463</v>
       </c>
       <c r="B466" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.3">
@@ -6625,7 +6757,7 @@
         <v>465</v>
       </c>
       <c r="B468" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.3">
@@ -6641,7 +6773,7 @@
         <v>467</v>
       </c>
       <c r="B470" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.3">
@@ -6649,10 +6781,10 @@
         <v>468</v>
       </c>
       <c r="B471" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C471" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.3">
@@ -6660,7 +6792,7 @@
         <v>469</v>
       </c>
       <c r="B472" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.3">
@@ -6668,7 +6800,7 @@
         <v>470</v>
       </c>
       <c r="B473" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.3">
@@ -6676,7 +6808,7 @@
         <v>471</v>
       </c>
       <c r="B474" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.3">
@@ -6684,10 +6816,10 @@
         <v>472</v>
       </c>
       <c r="B475" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C475" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.3">
@@ -6695,7 +6827,7 @@
         <v>473</v>
       </c>
       <c r="B476" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.3">
@@ -6711,7 +6843,7 @@
         <v>475</v>
       </c>
       <c r="B478" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.3">
@@ -6719,7 +6851,7 @@
         <v>476</v>
       </c>
       <c r="B479" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.3">
@@ -6727,7 +6859,7 @@
         <v>477</v>
       </c>
       <c r="B480" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.3">
@@ -6735,7 +6867,7 @@
         <v>478</v>
       </c>
       <c r="B481" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.3">
@@ -6751,7 +6883,7 @@
         <v>480</v>
       </c>
       <c r="B483" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.3">
@@ -6772,7 +6904,7 @@
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A486" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B486" t="s">
         <v>486</v>
@@ -6780,7 +6912,7 @@
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B487" t="s">
         <v>166</v>
@@ -6788,7 +6920,7 @@
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A488" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B488" t="s">
         <v>166</v>
@@ -6796,7 +6928,7 @@
     </row>
     <row r="489" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A489" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B489" t="s">
         <v>160</v>
@@ -6804,15 +6936,15 @@
     </row>
     <row r="490" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A490" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B490" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A491" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B491" t="s">
         <v>486</v>
@@ -6820,7 +6952,7 @@
     </row>
     <row r="492" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B492" t="s">
         <v>486</v>
@@ -6828,7 +6960,7 @@
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B493" t="s">
         <v>486</v>
@@ -6836,7 +6968,7 @@
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B494" t="s">
         <v>166</v>
@@ -6844,26 +6976,26 @@
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B495" t="s">
         <v>166</v>
       </c>
       <c r="C495" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B496" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B497" t="s">
         <v>485</v>
@@ -6871,18 +7003,18 @@
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B498" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C498" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B499" t="s">
         <v>485</v>
@@ -6890,61 +7022,61 @@
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B500" t="s">
         <v>160</v>
       </c>
       <c r="C500" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="501" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B501" t="s">
         <v>160</v>
       </c>
       <c r="C501" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B502" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B503" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="504" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B504" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B505" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="506" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B506" t="s">
         <v>166</v>
@@ -6952,7 +7084,7 @@
     </row>
     <row r="507" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B507" t="s">
         <v>486</v>
@@ -6960,29 +7092,29 @@
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B508" t="s">
         <v>166</v>
       </c>
       <c r="C508" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="509" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A509" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B509" t="s">
         <v>160</v>
       </c>
       <c r="C509" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="510" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B510" t="s">
         <v>160</v>
@@ -6990,7 +7122,7 @@
     </row>
     <row r="511" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B511" t="s">
         <v>160</v>
@@ -6998,45 +7130,45 @@
     </row>
     <row r="512" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A512" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B512" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C512" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="513" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B513" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="514" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B514" t="s">
         <v>486</v>
       </c>
       <c r="C514" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="515" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B515" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="516" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B516" t="s">
         <v>486</v>
@@ -7044,15 +7176,15 @@
     </row>
     <row r="517" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A517" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B517" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="518" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A518" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B518" t="s">
         <v>258</v>
@@ -7060,7 +7192,7 @@
     </row>
     <row r="519" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A519" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B519" t="s">
         <v>486</v>
@@ -7068,7 +7200,7 @@
     </row>
     <row r="520" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A520" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B520" t="s">
         <v>160</v>
@@ -7076,15 +7208,15 @@
     </row>
     <row r="521" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A521" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B521" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="522" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A522" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B522" t="s">
         <v>166</v>
@@ -7092,18 +7224,18 @@
     </row>
     <row r="523" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A523" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B523" t="s">
         <v>166</v>
       </c>
       <c r="C523" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="524" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A524" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B524" t="s">
         <v>7</v>
@@ -7111,15 +7243,15 @@
     </row>
     <row r="525" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A525" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B525" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="526" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A526" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B526" t="s">
         <v>486</v>
@@ -7127,45 +7259,45 @@
     </row>
     <row r="527" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A527" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B527" t="s">
         <v>363</v>
       </c>
       <c r="C527" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="528" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A528" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B528" t="s">
         <v>363</v>
       </c>
       <c r="C528" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="529" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A529" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B529" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="530" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A530" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B530" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="531" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A531" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B531" t="s">
         <v>160</v>
@@ -7173,7 +7305,7 @@
     </row>
     <row r="532" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A532" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B532" t="s">
         <v>160</v>
@@ -7181,7 +7313,7 @@
     </row>
     <row r="533" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A533" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B533" t="s">
         <v>166</v>
@@ -7189,15 +7321,15 @@
     </row>
     <row r="534" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A534" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B534" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="535" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A535" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B535" t="s">
         <v>486</v>
@@ -7205,7 +7337,7 @@
     </row>
     <row r="536" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A536" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B536" t="s">
         <v>166</v>
@@ -7213,7 +7345,7 @@
     </row>
     <row r="537" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A537" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B537" t="s">
         <v>166</v>
@@ -7221,23 +7353,23 @@
     </row>
     <row r="538" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A538" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B538" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="539" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A539" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B539" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="540" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A540" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B540" t="s">
         <v>160</v>
@@ -7245,15 +7377,15 @@
     </row>
     <row r="541" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A541" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B541" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="542" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A542" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B542" t="s">
         <v>486</v>
@@ -7261,29 +7393,29 @@
     </row>
     <row r="543" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A543" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B543" t="s">
         <v>486</v>
       </c>
       <c r="C543" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="544" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A544" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B544" t="s">
         <v>80</v>
       </c>
       <c r="C544" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="545" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A545" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B545" t="s">
         <v>166</v>
@@ -7291,7 +7423,7 @@
     </row>
     <row r="546" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A546" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B546" t="s">
         <v>166</v>
@@ -7299,7 +7431,7 @@
     </row>
     <row r="547" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A547" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B547" t="s">
         <v>486</v>
@@ -7307,18 +7439,18 @@
     </row>
     <row r="548" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A548" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B548" t="s">
         <v>363</v>
       </c>
       <c r="C548" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="549" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A549" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B549" t="s">
         <v>166</v>
@@ -7326,31 +7458,31 @@
     </row>
     <row r="550" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A550" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B550" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="551" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A551" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B551" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="552" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A552" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B552" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="553" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A553" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B553" t="s">
         <v>486</v>
@@ -7358,7 +7490,7 @@
     </row>
     <row r="554" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A554" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B554" t="s">
         <v>486</v>
@@ -7366,7 +7498,7 @@
     </row>
     <row r="555" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A555" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B555" t="s">
         <v>486</v>
@@ -7374,58 +7506,58 @@
     </row>
     <row r="556" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A556" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B556" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="557" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A557" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B557" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="558" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A558" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B558" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="559" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A559" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B559" t="s">
         <v>80</v>
       </c>
       <c r="C559" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="560" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A560" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B560" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="561" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A561" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B561" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="562" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A562" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B562" t="s">
         <v>166</v>
@@ -7433,23 +7565,23 @@
     </row>
     <row r="563" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A563" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B563" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="564" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A564" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B564" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="565" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A565" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B565" t="s">
         <v>486</v>
@@ -7457,39 +7589,39 @@
     </row>
     <row r="566" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A566" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B566" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="567" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A567" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B567" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="568" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A568" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B568" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="569" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A569" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B569" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="570" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A570" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B570" t="s">
         <v>258</v>
@@ -7497,7 +7629,7 @@
     </row>
     <row r="571" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A571" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B571" t="s">
         <v>166</v>
@@ -7505,7 +7637,7 @@
     </row>
     <row r="572" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A572" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B572" t="s">
         <v>486</v>
@@ -7513,64 +7645,64 @@
     </row>
     <row r="573" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A573" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B573" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="574" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A574" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B574" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="575" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A575" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B575" t="s">
         <v>8</v>
       </c>
       <c r="C575" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="576" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A576" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B576" t="s">
         <v>160</v>
       </c>
       <c r="C576" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="577" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A577" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B577" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
       <c r="C577" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="578" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A578" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B578" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="579" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A579" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B579" t="s">
         <v>8</v>
@@ -7578,15 +7710,15 @@
     </row>
     <row r="580" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A580" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B580" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="581" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A581" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B581" t="s">
         <v>166</v>
@@ -7594,7 +7726,7 @@
     </row>
     <row r="582" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A582" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B582" t="s">
         <v>166</v>
@@ -7602,18 +7734,18 @@
     </row>
     <row r="583" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A583" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B583" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C583" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="584" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B584" t="s">
         <v>486</v>
@@ -7621,7 +7753,7 @@
     </row>
     <row r="585" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B585" t="s">
         <v>486</v>
@@ -7629,7 +7761,7 @@
     </row>
     <row r="586" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A586" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B586" t="s">
         <v>486</v>
@@ -7637,7 +7769,7 @@
     </row>
     <row r="587" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A587" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B587" t="s">
         <v>166</v>
@@ -7645,15 +7777,15 @@
     </row>
     <row r="588" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A588" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B588" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="589" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A589" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B589" t="s">
         <v>486</v>
@@ -7661,7 +7793,7 @@
     </row>
     <row r="590" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A590" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B590" t="s">
         <v>166</v>
@@ -7669,7 +7801,7 @@
     </row>
     <row r="591" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A591" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B591" t="s">
         <v>485</v>
@@ -7677,7 +7809,7 @@
     </row>
     <row r="592" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A592" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B592" t="s">
         <v>160</v>
@@ -7685,37 +7817,37 @@
     </row>
     <row r="593" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A593" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B593" t="s">
         <v>166</v>
       </c>
       <c r="C593" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="594" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A594" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B594" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="595" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A595" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B595" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C595" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="596" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A596" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B596" t="s">
         <v>166</v>
@@ -7723,7 +7855,7 @@
     </row>
     <row r="597" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A597" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B597" t="s">
         <v>486</v>
@@ -7731,15 +7863,15 @@
     </row>
     <row r="598" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A598" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B598" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="599" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A599" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B599" t="s">
         <v>166</v>
@@ -7747,7 +7879,7 @@
     </row>
     <row r="600" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A600" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B600" t="s">
         <v>485</v>
@@ -7755,7 +7887,7 @@
     </row>
     <row r="601" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A601" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B601" t="s">
         <v>485</v>
@@ -7763,15 +7895,15 @@
     </row>
     <row r="602" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A602" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B602" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="603" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A603" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B603" t="s">
         <v>486</v>
@@ -7779,7 +7911,7 @@
     </row>
     <row r="604" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A604" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B604" t="s">
         <v>485</v>
@@ -7787,7 +7919,7 @@
     </row>
     <row r="605" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A605" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B605" t="s">
         <v>485</v>
@@ -7795,7 +7927,7 @@
     </row>
     <row r="606" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A606" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B606" t="s">
         <v>485</v>
@@ -7803,26 +7935,26 @@
     </row>
     <row r="607" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A607" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B607" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="608" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A608" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B608" t="s">
         <v>160</v>
       </c>
       <c r="C608" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="609" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A609" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B609" t="s">
         <v>166</v>
@@ -7830,7 +7962,7 @@
     </row>
     <row r="610" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A610" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B610" t="s">
         <v>363</v>
@@ -7838,7 +7970,7 @@
     </row>
     <row r="611" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A611" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B611" t="s">
         <v>363</v>
@@ -7846,34 +7978,34 @@
     </row>
     <row r="612" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A612" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B612" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="613" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A613" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B613" t="s">
         <v>160</v>
       </c>
       <c r="C613" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="614" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A614" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B614" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="615" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A615" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B615" t="s">
         <v>7</v>
@@ -7881,7 +8013,7 @@
     </row>
     <row r="616" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A616" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B616" t="s">
         <v>486</v>
@@ -7889,15 +8021,15 @@
     </row>
     <row r="617" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A617" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B617" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="618" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A618" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B618" t="s">
         <v>486</v>
@@ -7905,7 +8037,7 @@
     </row>
     <row r="619" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A619" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B619" t="s">
         <v>166</v>
@@ -7913,7 +8045,7 @@
     </row>
     <row r="620" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A620" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B620" t="s">
         <v>486</v>
@@ -7921,7 +8053,7 @@
     </row>
     <row r="621" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A621" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B621" t="s">
         <v>160</v>
@@ -7929,7 +8061,7 @@
     </row>
     <row r="622" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A622" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B622" t="s">
         <v>80</v>
@@ -7937,83 +8069,83 @@
     </row>
     <row r="623" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A623" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B623" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C623" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="624" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A624" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B624" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C624" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="625" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A625" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B625" t="s">
         <v>486</v>
       </c>
       <c r="C625" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="626" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A626" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B626" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="627" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A627" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B627" t="s">
         <v>166</v>
       </c>
       <c r="C627" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="628" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A628" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B628" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="629" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A629" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B629" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="630" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A630" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B630" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="631" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A631" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B631" t="s">
         <v>166</v>
@@ -8021,15 +8153,15 @@
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A632" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B632" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="633" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A633" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B633" t="s">
         <v>486</v>
@@ -8037,7 +8169,7 @@
     </row>
     <row r="634" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A634" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B634" t="s">
         <v>160</v>
@@ -8045,7 +8177,7 @@
     </row>
     <row r="635" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A635" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B635" t="s">
         <v>363</v>
@@ -8053,15 +8185,15 @@
     </row>
     <row r="636" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A636" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B636" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="637" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A637" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B637" t="s">
         <v>486</v>
@@ -8069,86 +8201,86 @@
     </row>
     <row r="638" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A638" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B638" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="639" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A639" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B639" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="640" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A640" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B640" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
       <c r="C640" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="641" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A641" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B641" t="s">
         <v>486</v>
       </c>
       <c r="C641" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="642" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A642" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B642" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C642" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="643" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A643" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B643" t="s">
         <v>258</v>
       </c>
       <c r="C643" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="644" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A644" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B644" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="645" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A645" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B645" t="s">
         <v>160</v>
       </c>
       <c r="C645" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="646" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A646" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B646" t="s">
         <v>485</v>
@@ -8156,31 +8288,31 @@
     </row>
     <row r="647" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A647" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B647" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="648" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A648" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B648" t="s">
-        <v>763</v>
+        <v>143</v>
       </c>
     </row>
     <row r="649" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A649" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B649" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="650" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A650" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B650" t="s">
         <v>486</v>
@@ -8188,7 +8320,7 @@
     </row>
     <row r="651" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A651" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B651" t="s">
         <v>166</v>
@@ -8196,7 +8328,7 @@
     </row>
     <row r="652" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A652" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B652" t="s">
         <v>7</v>
@@ -8204,7 +8336,7 @@
     </row>
     <row r="653" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A653" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B653" t="s">
         <v>486</v>
@@ -8212,7 +8344,7 @@
     </row>
     <row r="654" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A654" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B654" t="s">
         <v>486</v>
@@ -8220,7 +8352,7 @@
     </row>
     <row r="655" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A655" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B655" t="s">
         <v>166</v>
@@ -8228,18 +8360,18 @@
     </row>
     <row r="656" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A656" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B656" t="s">
         <v>363</v>
       </c>
       <c r="C656" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="657" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A657" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B657" t="s">
         <v>8</v>
@@ -8247,50 +8379,50 @@
     </row>
     <row r="658" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A658" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B658" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="659" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A659" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B659" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="660" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A660" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B660" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C660" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="661" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A661" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B661" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="662" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A662" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B662" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="663" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A663" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B663" t="s">
         <v>166</v>
@@ -8298,7 +8430,7 @@
     </row>
     <row r="664" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A664" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B664" t="s">
         <v>166</v>
@@ -8306,39 +8438,39 @@
     </row>
     <row r="665" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A665" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B665" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="666" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A666" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B666" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="667" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A667" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B667" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="668" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A668" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B668" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="669" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A669" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B669" t="s">
         <v>485</v>
@@ -8346,32 +8478,409 @@
     </row>
     <row r="670" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A670" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B670" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="671" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A671" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B671" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="672" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A672" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B672" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C672" t="s">
-        <v>762</v>
+        <v>761</v>
+      </c>
+    </row>
+    <row r="673" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A673" t="s">
+        <v>691</v>
+      </c>
+      <c r="B673" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="674" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A674" t="s">
+        <v>763</v>
+      </c>
+      <c r="B674" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="675" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A675" t="s">
+        <v>764</v>
+      </c>
+      <c r="B675" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="676" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A676" t="s">
+        <v>486</v>
+      </c>
+      <c r="B676" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="677" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A677" t="s">
+        <v>765</v>
+      </c>
+      <c r="B677" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="678" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A678" t="s">
+        <v>766</v>
+      </c>
+      <c r="B678" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="679" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A679" t="s">
+        <v>767</v>
+      </c>
+      <c r="B679" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="680" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A680" t="s">
+        <v>768</v>
+      </c>
+      <c r="B680" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="681" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A681" t="s">
+        <v>769</v>
+      </c>
+      <c r="B681" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="682" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A682" t="s">
+        <v>770</v>
+      </c>
+      <c r="B682" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="683" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A683" t="s">
+        <v>771</v>
+      </c>
+      <c r="B683" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A684" t="s">
+        <v>772</v>
+      </c>
+      <c r="B684" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="685" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A685" t="s">
+        <v>773</v>
+      </c>
+      <c r="B685" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A686" t="s">
+        <v>774</v>
+      </c>
+      <c r="B686" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A687" t="s">
+        <v>775</v>
+      </c>
+      <c r="B687" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="688" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A688" t="s">
+        <v>776</v>
+      </c>
+      <c r="B688" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="689" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A689" t="s">
+        <v>777</v>
+      </c>
+      <c r="B689" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="690" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A690" t="s">
+        <v>778</v>
+      </c>
+      <c r="B690" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="691" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A691" t="s">
+        <v>779</v>
+      </c>
+      <c r="B691" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="692" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A692" t="s">
+        <v>780</v>
+      </c>
+      <c r="B692" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="693" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A693" t="s">
+        <v>781</v>
+      </c>
+      <c r="B693" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="694" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A694" t="s">
+        <v>782</v>
+      </c>
+      <c r="B694" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="695" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A695" t="s">
+        <v>285</v>
+      </c>
+      <c r="B695" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="696" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A696" t="s">
+        <v>783</v>
+      </c>
+      <c r="B696" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="697" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A697" t="s">
+        <v>784</v>
+      </c>
+      <c r="B697" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="698" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A698" t="s">
+        <v>785</v>
+      </c>
+      <c r="B698" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="699" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A699" t="s">
+        <v>786</v>
+      </c>
+      <c r="B699" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="700" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A700" t="s">
+        <v>787</v>
+      </c>
+      <c r="B700" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="701" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A701" t="s">
+        <v>788</v>
+      </c>
+      <c r="B701" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="702" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A702" t="s">
+        <v>789</v>
+      </c>
+      <c r="B702" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="703" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A703" t="s">
+        <v>790</v>
+      </c>
+      <c r="B703" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="704" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A704" t="s">
+        <v>791</v>
+      </c>
+      <c r="B704" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="705" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A705" t="s">
+        <v>792</v>
+      </c>
+      <c r="B705" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="706" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A706" t="s">
+        <v>793</v>
+      </c>
+      <c r="B706" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="707" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A707" t="s">
+        <v>794</v>
+      </c>
+      <c r="B707" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A708" t="s">
+        <v>795</v>
+      </c>
+      <c r="B708" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="709" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A709" t="s">
+        <v>796</v>
+      </c>
+      <c r="B709" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="710" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A710" t="s">
+        <v>797</v>
+      </c>
+      <c r="B710" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="711" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A711" t="s">
+        <v>799</v>
+      </c>
+      <c r="B711" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="712" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A712" t="s">
+        <v>800</v>
+      </c>
+      <c r="B712" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="713" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A713" t="s">
+        <v>238</v>
+      </c>
+      <c r="B713" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="714" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A714" t="s">
+        <v>801</v>
+      </c>
+      <c r="B714" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="715" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A715" t="s">
+        <v>802</v>
+      </c>
+      <c r="B715" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="716" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A716" t="s">
+        <v>803</v>
+      </c>
+      <c r="B716" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="717" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A717" t="s">
+        <v>214</v>
+      </c>
+      <c r="B717" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="718" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A718" t="s">
+        <v>804</v>
+      </c>
+      <c r="B718" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="719" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A719" t="s">
+        <v>805</v>
+      </c>
+      <c r="B719" t="s">
+        <v>487</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B672" xr:uid="{015A9F8D-F621-4F22-B236-0DC5469AB275}"/>
   <hyperlinks>
     <hyperlink ref="C39" r:id="rId1" xr:uid="{F1047358-1DD7-4A87-B83B-B851DA7CA0AC}"/>
     <hyperlink ref="C475" r:id="rId2" xr:uid="{9C1D8F10-B434-4F42-9981-D559EDD53BC2}"/>

</xml_diff>